<commit_message>
initializer fixing rails dfault cuasing association error
</commit_message>
<xml_diff>
--- a/spec/fixtures/dummy_sheet.xlsx
+++ b/spec/fixtures/dummy_sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15620" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15620" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Vision" sheetId="1" r:id="rId1"/>
@@ -553,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -629,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>